<commit_message>
adjust remote DB IP info for deployment
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="20415" windowHeight="7560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="20415" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="3" r:id="rId1"/>
@@ -33,56 +33,56 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>localhost</t>
+    <t>速度偏差</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>导航X坐标下限(km)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>导航X坐标上限(km)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>导航Y坐标下限(km)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>导航Y坐标上限(km)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>导航Z坐标下限(km)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞行速度(m/sec)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>导航Z坐标上限(km)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>安全距离夹角</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>预设撞击时间间隔(sec)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.10.2.42</t>
     <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>速度偏差</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>导航X坐标下限(km)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>导航X坐标上限(km)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>导航Y坐标下限(km)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>导航Y坐标上限(km)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>导航Z坐标下限(km)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>飞行速度(m/sec)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>导航Z坐标上限(km)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>安全距离夹角</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>预设撞击时间间隔(sec)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -1110,7 +1110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1122,15 +1122,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="5">
         <v>235</v>
@@ -1138,7 +1138,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="6">
         <v>0.1</v>
@@ -1146,7 +1146,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5">
         <v>-5</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="5">
         <v>5</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>-5</v>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="5">
         <v>5</v>
@@ -1178,7 +1178,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="5">
         <v>3</v>
@@ -1194,7 +1194,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="7">
         <v>60</v>
@@ -1202,7 +1202,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="7">
         <v>90</v>

</xml_diff>